<commit_message>
inclusao de webofscience - capturei 80 - insercao de 10
</commit_message>
<xml_diff>
--- a/experiment_1/todo_francisco.xlsx
+++ b/experiment_1/todo_francisco.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Erica\hybrid_strategy\experiment_1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="581">
   <si>
     <t>A case study comparing defect profiles of a reused framework and of applications reusing it</t>
   </si>
@@ -2904,12 +2909,18 @@
   <si>
     <t>acm2015</t>
   </si>
+  <si>
+    <t xml:space="preserve">IT portfolio decision-making in local governments: Rationality, politics, intuition and coincidences </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The impact of global dispersion on coordination, team performance and software quality - A systematic literature review </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2925,13 +2936,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2958,27 +2995,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3016,9 +3068,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3050,9 +3102,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3084,9 +3137,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3259,14 +3313,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D289"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="109.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -3277,7 +3338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3291,7 +3352,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3305,7 +3366,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3319,7 +3380,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3333,7 +3394,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3347,7 +3408,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3361,7 +3422,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3375,7 +3436,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3389,7 +3450,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3403,7 +3464,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3417,7 +3478,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3431,7 +3492,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3445,7 +3506,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3459,7 +3520,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3473,7 +3534,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3487,7 +3548,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3501,7 +3562,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3515,7 +3576,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3529,7 +3590,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3543,7 +3604,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3557,7 +3618,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3571,7 +3632,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3585,7 +3646,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3599,7 +3660,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3613,7 +3674,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3627,7 +3688,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3641,7 +3702,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3655,7 +3716,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3669,7 +3730,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3683,7 +3744,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3697,7 +3758,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3711,7 +3772,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3725,7 +3786,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3739,7 +3800,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3753,7 +3814,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3767,7 +3828,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3781,7 +3842,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3795,7 +3856,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3809,7 +3870,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3823,7 +3884,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3837,7 +3898,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3851,7 +3912,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3865,7 +3926,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3879,7 +3940,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3893,7 +3954,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3907,7 +3968,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3921,7 +3982,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3935,7 +3996,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3949,7 +4010,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3963,7 +4024,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3977,7 +4038,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3991,7 +4052,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4005,7 +4066,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4019,7 +4080,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4033,7 +4094,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4047,7 +4108,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4061,7 +4122,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4075,7 +4136,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4089,7 +4150,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4103,7 +4164,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4117,7 +4178,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4131,7 +4192,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4145,7 +4206,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4159,7 +4220,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4173,7 +4234,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4187,7 +4248,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4201,7 +4262,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4215,7 +4276,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4229,7 +4290,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4243,7 +4304,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4257,7 +4318,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4271,7 +4332,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4285,7 +4346,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4299,7 +4360,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4313,7 +4374,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4327,7 +4388,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4341,7 +4402,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4355,7 +4416,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4369,7 +4430,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4383,7 +4444,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4397,7 +4458,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4411,7 +4472,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4425,7 +4486,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4439,7 +4500,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4453,7 +4514,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4467,7 +4528,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4481,7 +4542,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4495,7 +4556,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4509,7 +4570,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4523,7 +4584,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4537,7 +4598,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4551,7 +4612,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4565,7 +4626,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4579,7 +4640,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4593,7 +4654,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4607,7 +4668,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4621,7 +4682,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4635,7 +4696,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4649,7 +4710,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4663,7 +4724,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4677,7 +4738,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4691,7 +4752,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4705,7 +4766,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4719,7 +4780,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4733,7 +4794,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4747,7 +4808,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4761,7 +4822,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4775,7 +4836,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4789,7 +4850,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4803,7 +4864,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4817,7 +4878,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4831,7 +4892,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4845,7 +4906,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4859,7 +4920,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4873,7 +4934,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4887,7 +4948,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4901,7 +4962,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4915,25 +4976,25 @@
         <v>576</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C119" t="s">
         <v>405</v>
       </c>
-      <c r="D119" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="D119" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C120" t="s">
@@ -4943,11 +5004,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C121" t="s">
@@ -4957,11 +5018,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C122" t="s">
@@ -4971,11 +5032,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C123" t="s">
@@ -4985,11 +5046,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C124" t="s">
@@ -4999,11 +5060,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C125" t="s">
@@ -5013,11 +5074,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C126" t="s">
@@ -5027,11 +5088,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C127" t="s">
@@ -5041,11 +5102,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C128" t="s">
@@ -5055,11 +5116,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C129" t="s">
@@ -5069,11 +5130,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C130" t="s">
@@ -5083,11 +5144,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="4" t="s">
         <v>129</v>
       </c>
       <c r="C131" t="s">
@@ -5097,11 +5158,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C132" t="s">
@@ -5111,11 +5172,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C133" t="s">
@@ -5125,11 +5186,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C134" t="s">
@@ -5139,11 +5200,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C135" t="s">
@@ -5153,11 +5214,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C136" t="s">
@@ -5167,11 +5228,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C137" t="s">
@@ -5181,11 +5242,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C138" t="s">
@@ -5195,11 +5256,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C139" t="s">
@@ -5209,11 +5270,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C140" t="s">
@@ -5223,11 +5284,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C141" t="s">
@@ -5237,11 +5298,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C142" t="s">
@@ -5251,11 +5312,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C143" t="s">
@@ -5265,11 +5326,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C144" t="s">
@@ -5279,11 +5340,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C145" t="s">
@@ -5293,11 +5354,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="2" t="s">
         <v>144</v>
       </c>
       <c r="C146" t="s">
@@ -5307,11 +5368,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C147" t="s">
@@ -5321,11 +5382,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="2" t="s">
         <v>146</v>
       </c>
       <c r="C148" t="s">
@@ -5335,11 +5396,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="2" t="s">
         <v>147</v>
       </c>
       <c r="C149" t="s">
@@ -5349,11 +5410,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C150" t="s">
@@ -5363,11 +5424,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C151" t="s">
@@ -5377,11 +5438,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C152" t="s">
@@ -5391,11 +5452,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="2" t="s">
         <v>151</v>
       </c>
       <c r="C153" t="s">
@@ -5405,11 +5466,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C154" t="s">
@@ -5419,11 +5480,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C155" t="s">
@@ -5433,11 +5494,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C156" t="s">
@@ -5447,11 +5508,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C157" t="s">
@@ -5461,11 +5522,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C158" t="s">
@@ -5475,11 +5536,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C159" t="s">
@@ -5489,11 +5550,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C160" t="s">
@@ -5503,11 +5564,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="2" t="s">
         <v>159</v>
       </c>
       <c r="C161" t="s">
@@ -5517,11 +5578,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C162" t="s">
@@ -5531,11 +5592,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C163" t="s">
@@ -5545,11 +5606,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C164" t="s">
@@ -5559,11 +5620,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C165" t="s">
@@ -5573,11 +5634,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C166" t="s">
@@ -5587,11 +5648,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C167" t="s">
@@ -5601,11 +5662,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C168" t="s">
@@ -5615,11 +5676,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C169" t="s">
@@ -5629,11 +5690,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C170" t="s">
@@ -5643,11 +5704,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C171" t="s">
@@ -5657,11 +5718,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="4" t="s">
         <v>170</v>
       </c>
       <c r="C172" t="s">
@@ -5671,11 +5732,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C173" t="s">
@@ -5685,11 +5746,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C174" t="s">
@@ -5698,12 +5759,15 @@
       <c r="D174" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="175" spans="1:4">
+      <c r="E174" s="6" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C175" t="s">
@@ -5713,11 +5777,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C176" t="s">
@@ -5727,11 +5791,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C177" t="s">
@@ -5741,11 +5805,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C178" t="s">
@@ -5755,11 +5819,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C179" t="s">
@@ -5769,11 +5833,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C180" t="s">
@@ -5783,11 +5847,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C181" t="s">
@@ -5797,11 +5861,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C182" t="s">
@@ -5811,11 +5875,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C183" t="s">
@@ -5825,11 +5889,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C184" t="s">
@@ -5839,11 +5903,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C185" t="s">
@@ -5853,11 +5917,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C186" t="s">
@@ -5867,11 +5931,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C187" t="s">
@@ -5881,11 +5945,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="4" t="s">
         <v>186</v>
       </c>
       <c r="C188" t="s">
@@ -5895,11 +5959,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C189" t="s">
@@ -5909,11 +5973,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C190" t="s">
@@ -5923,11 +5987,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C191" t="s">
@@ -5937,11 +6001,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C192" t="s">
@@ -5951,11 +6015,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C193" t="s">
@@ -5964,12 +6028,15 @@
       <c r="D193" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
+      <c r="E193" s="6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C194" t="s">
@@ -5979,11 +6046,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C195" t="s">
@@ -5993,11 +6060,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C196" t="s">
@@ -6007,11 +6074,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C197" t="s">
@@ -6021,11 +6088,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C198" t="s">
@@ -6035,11 +6102,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C199" t="s">
@@ -6049,11 +6116,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C200" t="s">
@@ -6063,11 +6130,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C201" t="s">
@@ -6077,11 +6144,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C202" t="s">
@@ -6091,21 +6158,21 @@
         <v>577</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="D203" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
+      <c r="D203" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -6119,7 +6186,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -6133,7 +6200,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -6147,7 +6214,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -6161,7 +6228,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -6175,7 +6242,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -6189,7 +6256,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -6203,7 +6270,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -6217,7 +6284,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -6231,7 +6298,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -6245,7 +6312,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -6259,7 +6326,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -6273,7 +6340,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -6287,7 +6354,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -6301,7 +6368,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -6315,7 +6382,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -6329,7 +6396,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -6343,7 +6410,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -6357,7 +6424,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -6371,7 +6438,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -6385,7 +6452,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -6399,7 +6466,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -6413,7 +6480,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -6427,7 +6494,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -6441,7 +6508,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -6455,7 +6522,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -6469,7 +6536,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -6483,7 +6550,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -6497,7 +6564,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -6511,7 +6578,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -6525,7 +6592,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -6539,7 +6606,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -6553,7 +6620,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -6567,7 +6634,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -6581,7 +6648,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -6595,7 +6662,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="239" spans="1:4">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -6609,7 +6676,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -6623,7 +6690,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -6637,7 +6704,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="242" spans="1:4">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -6651,7 +6718,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="243" spans="1:4">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -6665,7 +6732,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -6679,7 +6746,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -6693,7 +6760,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -6707,7 +6774,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -6721,7 +6788,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -6735,7 +6802,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -6749,7 +6816,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -6763,7 +6830,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -6777,7 +6844,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="252" spans="1:4">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -6791,7 +6858,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -6805,7 +6872,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -6819,7 +6886,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="255" spans="1:4">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -6833,7 +6900,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="256" spans="1:4">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -6847,7 +6914,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -6861,7 +6928,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -6875,7 +6942,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -6889,7 +6956,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -6903,7 +6970,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -6917,7 +6984,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -6931,7 +6998,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -6945,7 +7012,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -6959,7 +7026,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="265" spans="1:4">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -6973,7 +7040,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="266" spans="1:4">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -6987,7 +7054,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="267" spans="1:4">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -7001,7 +7068,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="268" spans="1:4">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -7015,7 +7082,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="269" spans="1:4">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -7029,7 +7096,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="270" spans="1:4">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -7043,7 +7110,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="271" spans="1:4">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -7057,7 +7124,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="272" spans="1:4">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -7071,7 +7138,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="273" spans="1:4">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -7085,7 +7152,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -7099,7 +7166,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -7113,7 +7180,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -7127,7 +7194,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="277" spans="1:4">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -7141,7 +7208,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="278" spans="1:4">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -7155,7 +7222,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="279" spans="1:4">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -7169,7 +7236,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="280" spans="1:4">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -7183,7 +7250,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="281" spans="1:4">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -7197,7 +7264,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="282" spans="1:4">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -7211,7 +7278,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="283" spans="1:4">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -7225,7 +7292,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -7239,7 +7306,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="285" spans="1:4">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -7253,7 +7320,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -7267,7 +7334,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="287" spans="1:4">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -7281,7 +7348,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -7295,7 +7362,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -7310,6 +7377,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E174" r:id="rId1" display="http://apps-webofknowledge.ez24.periodicos.capes.gov.br/full_record.do?product=WOS&amp;search_mode=GeneralSearch&amp;qid=122&amp;SID=7BGZfA4AkT5bbJDeCzc&amp;page=1&amp;doc=1"/>
+    <hyperlink ref="E193" r:id="rId2" display="http://apps-webofknowledge.ez24.periodicos.capes.gov.br/full_record.do?product=WOS&amp;search_mode=GeneralSearch&amp;qid=44&amp;SID=8ERkgLkrMbolrxseli6&amp;page=1&amp;doc=1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
acm2015 - 57 estudos
</commit_message>
<xml_diff>
--- a/experiment_1/todo_francisco.xlsx
+++ b/experiment_1/todo_francisco.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="583">
   <si>
     <t>A case study comparing defect profiles of a reused framework and of applications reusing it</t>
   </si>
@@ -2914,6 +2914,12 @@
   </si>
   <si>
     <t xml:space="preserve">The impact of global dispersion on coordination, team performance and software quality - A systematic literature review </t>
+  </si>
+  <si>
+    <t>FALTAM 29 ACM</t>
+  </si>
+  <si>
+    <t>FALTAM 4 WEBOFSCIENCE</t>
   </si>
 </sst>
 </file>
@@ -2966,7 +2972,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3007,8 +3013,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3314,10 +3320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E289"/>
+  <dimension ref="A1:E292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="B291" sqref="B291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5759,7 +5765,7 @@
       <c r="D174" t="s">
         <v>577</v>
       </c>
-      <c r="E174" s="6" t="s">
+      <c r="E174" s="5" t="s">
         <v>579</v>
       </c>
     </row>
@@ -6028,7 +6034,7 @@
       <c r="D193" t="s">
         <v>577</v>
       </c>
-      <c r="E193" s="6" t="s">
+      <c r="E193" s="5" t="s">
         <v>580</v>
       </c>
     </row>
@@ -6162,13 +6168,13 @@
       <c r="A203" s="1">
         <v>201</v>
       </c>
-      <c r="B203" s="5" t="s">
+      <c r="B203" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C203" s="5" t="s">
+      <c r="C203" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="D203" s="5" t="s">
+      <c r="D203" s="3" t="s">
         <v>578</v>
       </c>
     </row>
@@ -6176,7 +6182,7 @@
       <c r="A204" s="1">
         <v>202</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="6" t="s">
         <v>202</v>
       </c>
       <c r="C204" t="s">
@@ -6190,7 +6196,7 @@
       <c r="A205" s="1">
         <v>203</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="6" t="s">
         <v>203</v>
       </c>
       <c r="C205" t="s">
@@ -6204,7 +6210,7 @@
       <c r="A206" s="1">
         <v>204</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="6" t="s">
         <v>204</v>
       </c>
       <c r="C206" t="s">
@@ -6218,7 +6224,7 @@
       <c r="A207" s="1">
         <v>205</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="6" t="s">
         <v>205</v>
       </c>
       <c r="C207" t="s">
@@ -6232,7 +6238,7 @@
       <c r="A208" s="1">
         <v>206</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="4" t="s">
         <v>206</v>
       </c>
       <c r="C208" t="s">
@@ -6246,7 +6252,7 @@
       <c r="A209" s="1">
         <v>207</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="6" t="s">
         <v>207</v>
       </c>
       <c r="C209" t="s">
@@ -6260,7 +6266,7 @@
       <c r="A210" s="1">
         <v>208</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="6" t="s">
         <v>208</v>
       </c>
       <c r="C210" t="s">
@@ -6274,7 +6280,7 @@
       <c r="A211" s="1">
         <v>209</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C211" t="s">
@@ -6288,7 +6294,7 @@
       <c r="A212" s="1">
         <v>210</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="6" t="s">
         <v>210</v>
       </c>
       <c r="C212" t="s">
@@ -6302,7 +6308,7 @@
       <c r="A213" s="1">
         <v>211</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="6" t="s">
         <v>211</v>
       </c>
       <c r="C213" t="s">
@@ -6316,7 +6322,7 @@
       <c r="A214" s="1">
         <v>212</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C214" t="s">
@@ -6330,7 +6336,7 @@
       <c r="A215" s="1">
         <v>213</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="6" t="s">
         <v>213</v>
       </c>
       <c r="C215" t="s">
@@ -6344,7 +6350,7 @@
       <c r="A216" s="1">
         <v>214</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="6" t="s">
         <v>214</v>
       </c>
       <c r="C216" t="s">
@@ -6358,7 +6364,7 @@
       <c r="A217" s="1">
         <v>215</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="6" t="s">
         <v>215</v>
       </c>
       <c r="C217" t="s">
@@ -6372,7 +6378,7 @@
       <c r="A218" s="1">
         <v>216</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="6" t="s">
         <v>216</v>
       </c>
       <c r="C218" t="s">
@@ -6386,7 +6392,7 @@
       <c r="A219" s="1">
         <v>217</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="6" t="s">
         <v>217</v>
       </c>
       <c r="C219" t="s">
@@ -6400,7 +6406,7 @@
       <c r="A220" s="1">
         <v>218</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="6" t="s">
         <v>218</v>
       </c>
       <c r="C220" t="s">
@@ -6414,7 +6420,7 @@
       <c r="A221" s="1">
         <v>219</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="6" t="s">
         <v>219</v>
       </c>
       <c r="C221" t="s">
@@ -6428,7 +6434,7 @@
       <c r="A222" s="1">
         <v>220</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C222" t="s">
@@ -6442,7 +6448,7 @@
       <c r="A223" s="1">
         <v>221</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B223" s="6" t="s">
         <v>221</v>
       </c>
       <c r="C223" t="s">
@@ -6456,7 +6462,7 @@
       <c r="A224" s="1">
         <v>222</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="6" t="s">
         <v>222</v>
       </c>
       <c r="C224" t="s">
@@ -6470,7 +6476,7 @@
       <c r="A225" s="1">
         <v>223</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="6" t="s">
         <v>223</v>
       </c>
       <c r="C225" t="s">
@@ -6484,7 +6490,7 @@
       <c r="A226" s="1">
         <v>224</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B226" s="4" t="s">
         <v>224</v>
       </c>
       <c r="C226" t="s">
@@ -6498,7 +6504,7 @@
       <c r="A227" s="1">
         <v>225</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B227" s="6" t="s">
         <v>225</v>
       </c>
       <c r="C227" t="s">
@@ -6512,7 +6518,7 @@
       <c r="A228" s="1">
         <v>226</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B228" s="6" t="s">
         <v>226</v>
       </c>
       <c r="C228" t="s">
@@ -6526,7 +6532,7 @@
       <c r="A229" s="1">
         <v>227</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B229" s="6" t="s">
         <v>227</v>
       </c>
       <c r="C229" t="s">
@@ -6540,7 +6546,7 @@
       <c r="A230" s="1">
         <v>228</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="4" t="s">
         <v>228</v>
       </c>
       <c r="C230" t="s">
@@ -6554,7 +6560,7 @@
       <c r="A231" s="1">
         <v>229</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B231" s="4" t="s">
         <v>229</v>
       </c>
       <c r="C231" t="s">
@@ -6568,7 +6574,7 @@
       <c r="A232" s="1">
         <v>230</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="6" t="s">
         <v>230</v>
       </c>
       <c r="C232" t="s">
@@ -6582,7 +6588,7 @@
       <c r="A233" s="1">
         <v>231</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B233" s="6" t="s">
         <v>231</v>
       </c>
       <c r="C233" t="s">
@@ -6596,7 +6602,7 @@
       <c r="A234" s="1">
         <v>232</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B234" s="4" t="s">
         <v>232</v>
       </c>
       <c r="C234" t="s">
@@ -6610,7 +6616,7 @@
       <c r="A235" s="1">
         <v>233</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B235" s="6" t="s">
         <v>233</v>
       </c>
       <c r="C235" t="s">
@@ -6624,7 +6630,7 @@
       <c r="A236" s="1">
         <v>234</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B236" s="4" t="s">
         <v>234</v>
       </c>
       <c r="C236" t="s">
@@ -6638,7 +6644,7 @@
       <c r="A237" s="1">
         <v>235</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B237" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C237" t="s">
@@ -6652,7 +6658,7 @@
       <c r="A238" s="1">
         <v>236</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B238" s="6" t="s">
         <v>236</v>
       </c>
       <c r="C238" t="s">
@@ -6666,7 +6672,7 @@
       <c r="A239" s="1">
         <v>237</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B239" s="6" t="s">
         <v>237</v>
       </c>
       <c r="C239" t="s">
@@ -6680,7 +6686,7 @@
       <c r="A240" s="1">
         <v>238</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B240" s="4" t="s">
         <v>238</v>
       </c>
       <c r="C240" t="s">
@@ -6694,7 +6700,7 @@
       <c r="A241" s="1">
         <v>239</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B241" s="4" t="s">
         <v>239</v>
       </c>
       <c r="C241" t="s">
@@ -6708,7 +6714,7 @@
       <c r="A242" s="1">
         <v>240</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B242" s="6" t="s">
         <v>240</v>
       </c>
       <c r="C242" t="s">
@@ -6722,7 +6728,7 @@
       <c r="A243" s="1">
         <v>241</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B243" s="6" t="s">
         <v>241</v>
       </c>
       <c r="C243" t="s">
@@ -6736,7 +6742,7 @@
       <c r="A244" s="1">
         <v>242</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B244" s="4" t="s">
         <v>242</v>
       </c>
       <c r="C244" t="s">
@@ -6750,7 +6756,7 @@
       <c r="A245" s="1">
         <v>243</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B245" s="4" t="s">
         <v>243</v>
       </c>
       <c r="C245" t="s">
@@ -6764,7 +6770,7 @@
       <c r="A246" s="1">
         <v>244</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B246" s="4" t="s">
         <v>244</v>
       </c>
       <c r="C246" t="s">
@@ -6778,7 +6784,7 @@
       <c r="A247" s="1">
         <v>245</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B247" s="6" t="s">
         <v>245</v>
       </c>
       <c r="C247" t="s">
@@ -6792,7 +6798,7 @@
       <c r="A248" s="1">
         <v>246</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B248" s="6" t="s">
         <v>246</v>
       </c>
       <c r="C248" t="s">
@@ -6806,7 +6812,7 @@
       <c r="A249" s="1">
         <v>247</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B249" s="6" t="s">
         <v>247</v>
       </c>
       <c r="C249" t="s">
@@ -6820,7 +6826,7 @@
       <c r="A250" s="1">
         <v>248</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B250" s="4" t="s">
         <v>248</v>
       </c>
       <c r="C250" t="s">
@@ -6834,7 +6840,7 @@
       <c r="A251" s="1">
         <v>249</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B251" s="4" t="s">
         <v>249</v>
       </c>
       <c r="C251" t="s">
@@ -6848,7 +6854,7 @@
       <c r="A252" s="1">
         <v>250</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B252" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C252" t="s">
@@ -6862,7 +6868,7 @@
       <c r="A253" s="1">
         <v>251</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B253" s="6" t="s">
         <v>251</v>
       </c>
       <c r="C253" t="s">
@@ -6876,7 +6882,7 @@
       <c r="A254" s="1">
         <v>252</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B254" s="6" t="s">
         <v>252</v>
       </c>
       <c r="C254" t="s">
@@ -6890,7 +6896,7 @@
       <c r="A255" s="1">
         <v>253</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B255" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C255" t="s">
@@ -6904,7 +6910,7 @@
       <c r="A256" s="1">
         <v>254</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B256" s="4" t="s">
         <v>254</v>
       </c>
       <c r="C256" t="s">
@@ -6918,7 +6924,7 @@
       <c r="A257" s="1">
         <v>255</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B257" s="4" t="s">
         <v>255</v>
       </c>
       <c r="C257" t="s">
@@ -6932,7 +6938,7 @@
       <c r="A258" s="1">
         <v>256</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B258" s="4" t="s">
         <v>256</v>
       </c>
       <c r="C258" t="s">
@@ -6946,7 +6952,7 @@
       <c r="A259" s="1">
         <v>257</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B259" s="6" t="s">
         <v>257</v>
       </c>
       <c r="C259" t="s">
@@ -6960,7 +6966,7 @@
       <c r="A260" s="1">
         <v>258</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B260" s="6" t="s">
         <v>258</v>
       </c>
       <c r="C260" t="s">
@@ -6974,7 +6980,7 @@
       <c r="A261" s="1">
         <v>259</v>
       </c>
-      <c r="B261" t="s">
+      <c r="B261" s="4" t="s">
         <v>259</v>
       </c>
       <c r="C261" t="s">
@@ -6988,7 +6994,7 @@
       <c r="A262" s="1">
         <v>260</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B262" s="6" t="s">
         <v>260</v>
       </c>
       <c r="C262" t="s">
@@ -7002,7 +7008,7 @@
       <c r="A263" s="1">
         <v>261</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B263" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C263" t="s">
@@ -7016,7 +7022,7 @@
       <c r="A264" s="1">
         <v>262</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B264" s="6" t="s">
         <v>262</v>
       </c>
       <c r="C264" t="s">
@@ -7030,7 +7036,7 @@
       <c r="A265" s="1">
         <v>263</v>
       </c>
-      <c r="B265" t="s">
+      <c r="B265" s="6" t="s">
         <v>263</v>
       </c>
       <c r="C265" t="s">
@@ -7044,7 +7050,7 @@
       <c r="A266" s="1">
         <v>264</v>
       </c>
-      <c r="B266" t="s">
+      <c r="B266" s="6" t="s">
         <v>264</v>
       </c>
       <c r="C266" t="s">
@@ -7058,7 +7064,7 @@
       <c r="A267" s="1">
         <v>265</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B267" s="6" t="s">
         <v>265</v>
       </c>
       <c r="C267" t="s">
@@ -7072,7 +7078,7 @@
       <c r="A268" s="1">
         <v>266</v>
       </c>
-      <c r="B268" t="s">
+      <c r="B268" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C268" t="s">
@@ -7086,7 +7092,7 @@
       <c r="A269" s="1">
         <v>267</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B269" s="6" t="s">
         <v>267</v>
       </c>
       <c r="C269" t="s">
@@ -7100,7 +7106,7 @@
       <c r="A270" s="1">
         <v>268</v>
       </c>
-      <c r="B270" t="s">
+      <c r="B270" s="6" t="s">
         <v>268</v>
       </c>
       <c r="C270" t="s">
@@ -7114,7 +7120,7 @@
       <c r="A271" s="1">
         <v>269</v>
       </c>
-      <c r="B271" t="s">
+      <c r="B271" s="4" t="s">
         <v>269</v>
       </c>
       <c r="C271" t="s">
@@ -7128,7 +7134,7 @@
       <c r="A272" s="1">
         <v>270</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B272" s="6" t="s">
         <v>270</v>
       </c>
       <c r="C272" t="s">
@@ -7142,7 +7148,7 @@
       <c r="A273" s="1">
         <v>271</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B273" s="4" t="s">
         <v>271</v>
       </c>
       <c r="C273" t="s">
@@ -7156,7 +7162,7 @@
       <c r="A274" s="1">
         <v>272</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B274" s="6" t="s">
         <v>272</v>
       </c>
       <c r="C274" t="s">
@@ -7170,7 +7176,7 @@
       <c r="A275" s="1">
         <v>273</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B275" s="4" t="s">
         <v>273</v>
       </c>
       <c r="C275" t="s">
@@ -7184,7 +7190,7 @@
       <c r="A276" s="1">
         <v>274</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B276" s="4" t="s">
         <v>274</v>
       </c>
       <c r="C276" t="s">
@@ -7198,7 +7204,7 @@
       <c r="A277" s="1">
         <v>275</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B277" s="6" t="s">
         <v>275</v>
       </c>
       <c r="C277" t="s">
@@ -7212,7 +7218,7 @@
       <c r="A278" s="1">
         <v>276</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B278" s="4" t="s">
         <v>276</v>
       </c>
       <c r="C278" t="s">
@@ -7226,7 +7232,7 @@
       <c r="A279" s="1">
         <v>277</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B279" s="6" t="s">
         <v>277</v>
       </c>
       <c r="C279" t="s">
@@ -7240,7 +7246,7 @@
       <c r="A280" s="1">
         <v>278</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B280" s="6" t="s">
         <v>278</v>
       </c>
       <c r="C280" t="s">
@@ -7254,7 +7260,7 @@
       <c r="A281" s="1">
         <v>279</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B281" s="6" t="s">
         <v>279</v>
       </c>
       <c r="C281" t="s">
@@ -7268,7 +7274,7 @@
       <c r="A282" s="1">
         <v>280</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B282" s="6" t="s">
         <v>280</v>
       </c>
       <c r="C282" t="s">
@@ -7282,7 +7288,7 @@
       <c r="A283" s="1">
         <v>281</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B283" s="6" t="s">
         <v>281</v>
       </c>
       <c r="C283" t="s">
@@ -7296,7 +7302,7 @@
       <c r="A284" s="1">
         <v>282</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B284" s="4" t="s">
         <v>282</v>
       </c>
       <c r="C284" t="s">
@@ -7310,7 +7316,7 @@
       <c r="A285" s="1">
         <v>283</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B285" s="6" t="s">
         <v>283</v>
       </c>
       <c r="C285" t="s">
@@ -7324,7 +7330,7 @@
       <c r="A286" s="1">
         <v>284</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B286" s="6" t="s">
         <v>284</v>
       </c>
       <c r="C286" t="s">
@@ -7338,7 +7344,7 @@
       <c r="A287" s="1">
         <v>285</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B287" s="4" t="s">
         <v>285</v>
       </c>
       <c r="C287" t="s">
@@ -7352,7 +7358,7 @@
       <c r="A288" s="1">
         <v>286</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B288" s="4" t="s">
         <v>286</v>
       </c>
       <c r="C288" t="s">
@@ -7366,7 +7372,7 @@
       <c r="A289" s="1">
         <v>287</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B289" s="6" t="s">
         <v>287</v>
       </c>
       <c r="C289" t="s">
@@ -7374,6 +7380,16 @@
       </c>
       <c r="D289" t="s">
         <v>578</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B291" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B292" t="s">
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sciencedirect2015 - 4 finais
</commit_message>
<xml_diff>
--- a/experiment_1/todo_francisco.xlsx
+++ b/experiment_1/todo_francisco.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="584">
   <si>
     <t>A case study comparing defect profiles of a reused framework and of applications reusing it</t>
   </si>
@@ -2919,7 +2919,10 @@
     <t>FALTAM 29 ACM</t>
   </si>
   <si>
-    <t>FALTAM 4 WEBOFSCIENCE</t>
+    <t>scholar</t>
+  </si>
+  <si>
+    <t>FALTAM 4 sciencedirect - ok encontrado no scholar</t>
   </si>
 </sst>
 </file>
@@ -2951,7 +2954,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2979,6 +2982,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3011,7 +3020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3022,6 +3031,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3329,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="B292" sqref="B292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5129,7 +5139,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5143,7 +5153,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5157,11 +5167,11 @@
         <v>577</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C131" t="s">
@@ -5170,8 +5180,11 @@
       <c r="D131" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5185,7 +5198,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5199,7 +5212,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5213,7 +5226,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5227,7 +5240,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5255,7 +5268,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5269,7 +5282,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5283,7 +5296,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5297,7 +5310,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5311,7 +5324,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5325,7 +5338,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5339,7 +5352,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5735,7 +5748,7 @@
       <c r="A172" s="1">
         <v>170</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B172" s="8" t="s">
         <v>170</v>
       </c>
       <c r="C172" t="s">
@@ -5822,7 +5835,7 @@
       <c r="A178" s="1">
         <v>176</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C178" t="s">
@@ -5962,7 +5975,7 @@
       <c r="A188" s="1">
         <v>186</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="8" t="s">
         <v>186</v>
       </c>
       <c r="C188" t="s">
@@ -6245,7 +6258,7 @@
       <c r="A208" s="1">
         <v>206</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="B208" s="8" t="s">
         <v>206</v>
       </c>
       <c r="C208" t="s">
@@ -6441,7 +6454,7 @@
       <c r="A222" s="1">
         <v>220</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="B222" s="8" t="s">
         <v>220</v>
       </c>
       <c r="C222" t="s">
@@ -6497,7 +6510,7 @@
       <c r="A226" s="1">
         <v>224</v>
       </c>
-      <c r="B226" s="4" t="s">
+      <c r="B226" s="8" t="s">
         <v>224</v>
       </c>
       <c r="C226" t="s">
@@ -6553,7 +6566,7 @@
       <c r="A230" s="1">
         <v>228</v>
       </c>
-      <c r="B230" s="4" t="s">
+      <c r="B230" s="8" t="s">
         <v>228</v>
       </c>
       <c r="C230" t="s">
@@ -6609,7 +6622,7 @@
       <c r="A234" s="1">
         <v>232</v>
       </c>
-      <c r="B234" s="4" t="s">
+      <c r="B234" s="8" t="s">
         <v>232</v>
       </c>
       <c r="C234" t="s">
@@ -6637,7 +6650,7 @@
       <c r="A236" s="1">
         <v>234</v>
       </c>
-      <c r="B236" s="4" t="s">
+      <c r="B236" s="8" t="s">
         <v>234</v>
       </c>
       <c r="C236" t="s">
@@ -6693,7 +6706,7 @@
       <c r="A240" s="1">
         <v>238</v>
       </c>
-      <c r="B240" s="4" t="s">
+      <c r="B240" s="8" t="s">
         <v>238</v>
       </c>
       <c r="C240" t="s">
@@ -6707,7 +6720,7 @@
       <c r="A241" s="1">
         <v>239</v>
       </c>
-      <c r="B241" s="4" t="s">
+      <c r="B241" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C241" t="s">
@@ -7391,7 +7404,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -7405,5 +7418,6 @@
     <hyperlink ref="E193" r:id="rId2" display="http://apps-webofknowledge.ez24.periodicos.capes.gov.br/full_record.do?product=WOS&amp;search_mode=GeneralSearch&amp;qid=44&amp;SID=8ERkgLkrMbolrxseli6&amp;page=1&amp;doc=1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
acm2015 - 27 restantes
</commit_message>
<xml_diff>
--- a/experiment_1/todo_francisco.xlsx
+++ b/experiment_1/todo_francisco.xlsx
@@ -2916,13 +2916,13 @@
     <t xml:space="preserve">The impact of global dispersion on coordination, team performance and software quality - A systematic literature review </t>
   </si>
   <si>
-    <t>FALTAM 29 ACM</t>
-  </si>
-  <si>
     <t>scholar</t>
   </si>
   <si>
-    <t>FALTAM 4 sciencedirect - ok encontrado no scholar</t>
+    <t>Não consegui encontrar 4 no sciencedirect. Encontrei no scholar</t>
+  </si>
+  <si>
+    <t>Não consegui encontrar 29 na acm. Encontrei no scholar</t>
   </si>
 </sst>
 </file>
@@ -3339,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="B292" sqref="B292"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="B255" sqref="B255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,7 +5181,7 @@
         <v>577</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -6762,7 +6762,7 @@
       <c r="A244" s="1">
         <v>242</v>
       </c>
-      <c r="B244" s="4" t="s">
+      <c r="B244" s="8" t="s">
         <v>242</v>
       </c>
       <c r="C244" t="s">
@@ -6776,7 +6776,7 @@
       <c r="A245" s="1">
         <v>243</v>
       </c>
-      <c r="B245" s="4" t="s">
+      <c r="B245" s="8" t="s">
         <v>243</v>
       </c>
       <c r="C245" t="s">
@@ -6790,7 +6790,7 @@
       <c r="A246" s="1">
         <v>244</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="B246" s="8" t="s">
         <v>244</v>
       </c>
       <c r="C246" t="s">
@@ -6846,7 +6846,7 @@
       <c r="A250" s="1">
         <v>248</v>
       </c>
-      <c r="B250" s="4" t="s">
+      <c r="B250" s="8" t="s">
         <v>248</v>
       </c>
       <c r="C250" t="s">
@@ -6860,7 +6860,7 @@
       <c r="A251" s="1">
         <v>249</v>
       </c>
-      <c r="B251" s="4" t="s">
+      <c r="B251" s="8" t="s">
         <v>249</v>
       </c>
       <c r="C251" t="s">
@@ -6930,7 +6930,7 @@
       <c r="A256" s="1">
         <v>254</v>
       </c>
-      <c r="B256" s="4" t="s">
+      <c r="B256" s="8" t="s">
         <v>254</v>
       </c>
       <c r="C256" t="s">
@@ -6944,7 +6944,7 @@
       <c r="A257" s="1">
         <v>255</v>
       </c>
-      <c r="B257" s="4" t="s">
+      <c r="B257" s="8" t="s">
         <v>255</v>
       </c>
       <c r="C257" t="s">
@@ -6958,7 +6958,7 @@
       <c r="A258" s="1">
         <v>256</v>
       </c>
-      <c r="B258" s="4" t="s">
+      <c r="B258" s="8" t="s">
         <v>256</v>
       </c>
       <c r="C258" t="s">
@@ -7000,7 +7000,7 @@
       <c r="A261" s="1">
         <v>259</v>
       </c>
-      <c r="B261" s="4" t="s">
+      <c r="B261" s="8" t="s">
         <v>259</v>
       </c>
       <c r="C261" t="s">
@@ -7028,7 +7028,7 @@
       <c r="A263" s="1">
         <v>261</v>
       </c>
-      <c r="B263" s="4" t="s">
+      <c r="B263" s="8" t="s">
         <v>261</v>
       </c>
       <c r="C263" t="s">
@@ -7098,7 +7098,7 @@
       <c r="A268" s="1">
         <v>266</v>
       </c>
-      <c r="B268" s="4" t="s">
+      <c r="B268" s="8" t="s">
         <v>266</v>
       </c>
       <c r="C268" t="s">
@@ -7140,7 +7140,7 @@
       <c r="A271" s="1">
         <v>269</v>
       </c>
-      <c r="B271" s="4" t="s">
+      <c r="B271" s="8" t="s">
         <v>269</v>
       </c>
       <c r="C271" t="s">
@@ -7168,7 +7168,7 @@
       <c r="A273" s="1">
         <v>271</v>
       </c>
-      <c r="B273" s="4" t="s">
+      <c r="B273" s="8" t="s">
         <v>271</v>
       </c>
       <c r="C273" t="s">
@@ -7196,7 +7196,7 @@
       <c r="A275" s="1">
         <v>273</v>
       </c>
-      <c r="B275" s="4" t="s">
+      <c r="B275" s="8" t="s">
         <v>273</v>
       </c>
       <c r="C275" t="s">
@@ -7210,7 +7210,7 @@
       <c r="A276" s="1">
         <v>274</v>
       </c>
-      <c r="B276" s="4" t="s">
+      <c r="B276" s="8" t="s">
         <v>274</v>
       </c>
       <c r="C276" t="s">
@@ -7238,7 +7238,7 @@
       <c r="A278" s="1">
         <v>276</v>
       </c>
-      <c r="B278" s="4" t="s">
+      <c r="B278" s="8" t="s">
         <v>276</v>
       </c>
       <c r="C278" t="s">
@@ -7322,7 +7322,7 @@
       <c r="A284" s="1">
         <v>282</v>
       </c>
-      <c r="B284" s="4" t="s">
+      <c r="B284" s="8" t="s">
         <v>282</v>
       </c>
       <c r="C284" t="s">
@@ -7364,7 +7364,7 @@
       <c r="A287" s="1">
         <v>285</v>
       </c>
-      <c r="B287" s="4" t="s">
+      <c r="B287" s="8" t="s">
         <v>285</v>
       </c>
       <c r="C287" t="s">
@@ -7378,7 +7378,7 @@
       <c r="A288" s="1">
         <v>286</v>
       </c>
-      <c r="B288" s="4" t="s">
+      <c r="B288" s="8" t="s">
         <v>286</v>
       </c>
       <c r="C288" t="s">
@@ -7403,13 +7403,13 @@
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B291" t="s">
+      <c r="B291" s="8" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B292" s="8" t="s">
         <v>583</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B292" t="s">
-        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
acm2015 - 4 encontrados
</commit_message>
<xml_diff>
--- a/experiment_1/todo_francisco.xlsx
+++ b/experiment_1/todo_francisco.xlsx
@@ -3339,8 +3339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="B255" sqref="B255"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>